<commit_message>
push changes to fix gender
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-mother-other-children.xlsx
+++ b/output/StructureDefinition-mother-other-children.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="340">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-06-23T12:11:34+01:00</t>
+    <t>2025-06-23T13:45:54+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -901,7 +901,10 @@
     <t>Needed for identification of the person, in combination with (at least) name and birth date.</t>
   </si>
   <si>
-    <t>http://nphcda.gov.ng/ig/fhir/ValueSet/ng-gender</t>
+    <t>The gender of a person used for administrative purposes.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/administrative-gender|4.0.1</t>
   </si>
   <si>
     <t>administrativeGender</t>
@@ -4838,9 +4841,11 @@
       <c r="X31" t="s" s="2">
         <v>205</v>
       </c>
-      <c r="Y31" s="2"/>
+      <c r="Y31" t="s" s="2">
+        <v>285</v>
+      </c>
       <c r="Z31" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AA31" t="s" s="2">
         <v>76</v>
@@ -4873,21 +4878,21 @@
         <v>97</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AL31" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -4910,13 +4915,13 @@
         <v>86</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -4967,7 +4972,7 @@
         <v>76</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>77</v>
@@ -4982,7 +4987,7 @@
         <v>97</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AL32" t="s" s="2">
         <v>76</v>
@@ -4993,10 +4998,10 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5019,17 +5024,17 @@
         <v>86</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="P33" t="s" s="2">
         <v>76</v>
@@ -5078,7 +5083,7 @@
         <v>76</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>77</v>
@@ -5093,21 +5098,21 @@
         <v>97</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="AL33" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5130,17 +5135,17 @@
         <v>76</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="P34" t="s" s="2">
         <v>76</v>
@@ -5189,7 +5194,7 @@
         <v>76</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>77</v>
@@ -5204,21 +5209,21 @@
         <v>97</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AL34" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5244,10 +5249,10 @@
         <v>266</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
@@ -5298,7 +5303,7 @@
         <v>76</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>77</v>
@@ -5313,10 +5318,10 @@
         <v>97</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="AM35" t="s" s="2">
         <v>76</v>
@@ -5324,10 +5329,10 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5350,19 +5355,19 @@
         <v>76</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="O36" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="P36" t="s" s="2">
         <v>76</v>
@@ -5411,7 +5416,7 @@
         <v>76</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>77</v>
@@ -5426,7 +5431,7 @@
         <v>97</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AL36" t="s" s="2">
         <v>76</v>
@@ -5437,10 +5442,10 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5546,10 +5551,10 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -5657,14 +5662,14 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s" s="2">
@@ -5686,16 +5691,16 @@
         <v>130</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="N39" t="s" s="2">
         <v>188</v>
       </c>
       <c r="O39" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="P39" t="s" s="2">
         <v>76</v>
@@ -5744,7 +5749,7 @@
         <v>76</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>77</v>
@@ -5770,10 +5775,10 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -5799,16 +5804,16 @@
         <v>170</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="O40" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="P40" t="s" s="2">
         <v>76</v>
@@ -5857,7 +5862,7 @@
         <v>76</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>85</v>
@@ -5872,7 +5877,7 @@
         <v>97</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>76</v>
@@ -5883,10 +5888,10 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -5912,16 +5917,16 @@
         <v>154</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="O41" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="P41" t="s" s="2">
         <v>76</v>
@@ -5970,7 +5975,7 @@
         <v>76</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>77</v>
@@ -5985,7 +5990,7 @@
         <v>97</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>76</v>

</xml_diff>